<commit_message>
Consulta API, Insercion DB, Reporte Excel en proceso
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B89DAF-D1AC-43DC-A915-CACA2137585E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="2"/>
+    <workbookView xWindow="1519" yWindow="1519" windowWidth="18850" windowHeight="9765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>Key</t>
   </si>
@@ -51,13 +52,49 @@
   </si>
   <si>
     <t>ShouldStopMasterAssetName</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://fakestoreapi.com/products</t>
+  </si>
+  <si>
+    <t>DB_Server</t>
+  </si>
+  <si>
+    <t>DB_Name</t>
+  </si>
+  <si>
+    <t>DB_User</t>
+  </si>
+  <si>
+    <t>DB_Pass</t>
+  </si>
+  <si>
+    <t>postgres</t>
+  </si>
+  <si>
+    <t>gabtrek</t>
+  </si>
+  <si>
+    <t>localhost</t>
+  </si>
+  <si>
+    <t>ReportPath</t>
+  </si>
+  <si>
+    <t>Data/Reportes/Reporte_{0}.xlsx</t>
+  </si>
+  <si>
+    <t>RPA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +109,22 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -92,14 +145,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -377,21 +434,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -402,7 +459,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -410,27 +467,83 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C10" s="2"/>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" display="http://localhost" xr:uid="{FB1F93FD-1D1D-41E4-9EF2-CA36BCC1C5E9}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{C59C6F6D-9BBF-4CD7-A50D-083D1D8EAE02}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C65160-A8E0-446E-AF4F-971CC91598A3}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+    <col min="2" max="2" width="35.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -449,7 +562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -457,7 +570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -472,14 +585,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36020AE9-9DBE-489C-A1AC-B86CE2043714}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="20.3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
FormUpload en procesos. Etapa final
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B89DAF-D1AC-43DC-A915-CACA2137585E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4104236D-41D5-4393-AB21-F29DE0CC522C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1519" yWindow="1519" windowWidth="18850" windowHeight="9765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Key</t>
   </si>
@@ -88,13 +88,25 @@
   </si>
   <si>
     <t>RPA</t>
+  </si>
+  <si>
+    <t>https://form.jotform.com/250753158727665</t>
+  </si>
+  <si>
+    <t>Form_URL</t>
+  </si>
+  <si>
+    <t>Colaborador</t>
+  </si>
+  <si>
+    <t>Gabriel Ballone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +139,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -149,11 +168,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -435,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -515,16 +535,34 @@
         <v>20</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
       <c r="C10" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" display="http://localhost" xr:uid="{FB1F93FD-1D1D-41E4-9EF2-CA36BCC1C5E9}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{C59C6F6D-9BBF-4CD7-A50D-083D1D8EAE02}"/>
+    <hyperlink ref="B9" r:id="rId3" xr:uid="{39298399-2935-45B5-9A19-CF4AD7852E06}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>